<commit_message>
modified the test cases and src files
</commit_message>
<xml_diff>
--- a/data/AI Grant Finding & Writing - Keywords_M2_TG.xlsx
+++ b/data/AI Grant Finding & Writing - Keywords_M2_TG.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -636,6 +636,42 @@
         </is>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Construction Safety and Compliance</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>abc</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Sustainable Building and Construction</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>xyz</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Sustainable Building and Construction</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>abc</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>